<commit_message>
changed the randomint range to be within range
</commit_message>
<xml_diff>
--- a/Stats Question.xlsx
+++ b/Stats Question.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pikak\CS\Stats_Study_Question\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8DF2706-BF47-4717-9F99-AB3E1BB69A1C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{541C17EB-8692-4997-AC4A-C796C15275D5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{E395EDCE-F408-40B2-8E9F-6BC6DF6B84F4}"/>
+    <workbookView xWindow="-14325" yWindow="3540" windowWidth="28800" windowHeight="15435" xr2:uid="{E395EDCE-F408-40B2-8E9F-6BC6DF6B84F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1097,7 +1097,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A163365-0FC8-491B-B183-69C051A468D2}">
   <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
       <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
@@ -1986,6 +1986,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000FBE23F23D6C404CAD5DE15B10DA803A" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9c0a2ea5eccded9113d6acc92c2e0eee">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="73decd86-39a4-49eb-910d-a9d7478bb842" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="95988c120be2346af9c3b7b357a780e1" ns3:_="">
     <xsd:import namespace="73decd86-39a4-49eb-910d-a9d7478bb842"/>
@@ -2143,15 +2152,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2159,6 +2159,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45F27491-F991-417B-A5F3-2092F2BFE652}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0CE6D41D-ABD0-43C8-8448-083F658CE12C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2172,14 +2180,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45F27491-F991-417B-A5F3-2092F2BFE652}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
added some quiz 6 stuff
</commit_message>
<xml_diff>
--- a/Stats Question.xlsx
+++ b/Stats Question.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pikak\CS\Stats_Study_Question\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{541C17EB-8692-4997-AC4A-C796C15275D5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02864EC5-6D84-4832-B072-1A2C2F496D29}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14325" yWindow="3540" windowWidth="28800" windowHeight="15435" xr2:uid="{E395EDCE-F408-40B2-8E9F-6BC6DF6B84F4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{E395EDCE-F408-40B2-8E9F-6BC6DF6B84F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="230">
   <si>
     <t>Question</t>
   </si>
@@ -124,12 +124,6 @@
 an example of</t>
   </si>
   <si>
-    <t>A sportswriter wants to know how strongly residents support building a new stadium downtown for the local major league soccer team. She prints a survey in her column and asks her readers to send in their response. One thousand readers sent in their response.
-Critics of the poll argue that the poll only sampled readers
-of her column and not all residents of the city. This is an
-example of</t>
-  </si>
-  <si>
     <t>Some common sources of nonsampling error in samples of human populations are</t>
   </si>
   <si>
@@ -741,6 +735,42 @@
   </si>
   <si>
     <t xml:space="preserve">    matching.</t>
+  </si>
+  <si>
+    <t>A sportswriter wants to know how strongly residents support building a new stadium downtown for the local major league soccer team. She prints a survey in her column and asks her readers to send in their response. One thousand readers sent in their response.
+Critics of the poll argue that the poll only sampled readers
+of her column and not all residents of the city. This is an example of</t>
+  </si>
+  <si>
+    <t>It is difficult to establish the causal link between cigarette smoking and lung cancer because</t>
+  </si>
+  <si>
+    <t>random allocation of subjects to smoking is unethical.</t>
+  </si>
+  <si>
+    <t>those who choose to smoke may be genetically at greater risk for lung cancer than those who don't choose to smoke.</t>
+  </si>
+  <si>
+    <t>experiments done on animals may not be valid for humans.</t>
+  </si>
+  <si>
+    <t>all of the above</t>
+  </si>
+  <si>
+    <t>A professor believes that students who smoke cigarettes tend to have lower grades. He collects data from 1326 randomly selected students at his university and discovers that, on average, students who smoke cigarettes do indeed tend to have lower grade point averages than students who do not smoke.
+This study was based on</t>
+  </si>
+  <si>
+    <t>a randomized comparative experiment.</t>
+  </si>
+  <si>
+    <t>a matched pairs experiment.</t>
+  </si>
+  <si>
+    <t>a voluntary response sample.</t>
+  </si>
+  <si>
+    <t>a probability sample.</t>
   </si>
 </sst>
 </file>
@@ -1095,21 +1125,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A163365-0FC8-491B-B183-69C051A468D2}">
-  <dimension ref="A1:M41"/>
+  <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="G50" sqref="G50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="55.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" customWidth="1"/>
+    <col min="3" max="3" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1132,852 +1162,889 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E3" t="s">
         <v>158</v>
-      </c>
-      <c r="B3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C3" t="s">
-        <v>81</v>
-      </c>
-      <c r="D3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E3" t="s">
-        <v>159</v>
       </c>
       <c r="G3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
+        <v>159</v>
+      </c>
+      <c r="C4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" t="s">
         <v>160</v>
       </c>
-      <c r="C4" t="s">
-        <v>82</v>
-      </c>
-      <c r="D4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E4" t="s">
-        <v>161</v>
-      </c>
       <c r="F4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>161</v>
+      </c>
+      <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5" t="s">
+        <v>119</v>
+      </c>
+      <c r="E5" t="s">
         <v>162</v>
-      </c>
-      <c r="B5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" t="s">
-        <v>83</v>
-      </c>
-      <c r="D5" t="s">
-        <v>120</v>
-      </c>
-      <c r="E5" t="s">
-        <v>163</v>
       </c>
       <c r="G5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D8" t="s">
+        <v>165</v>
+      </c>
+      <c r="E8" t="s">
         <v>166</v>
-      </c>
-      <c r="E8" t="s">
-        <v>167</v>
       </c>
       <c r="G8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F10" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E11" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F11" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>15</v>
       </c>
       <c r="B12" t="s">
+        <v>125</v>
+      </c>
+      <c r="C12" t="s">
+        <v>89</v>
+      </c>
+      <c r="D12" t="s">
         <v>126</v>
       </c>
-      <c r="C12" t="s">
-        <v>90</v>
-      </c>
-      <c r="D12" t="s">
-        <v>127</v>
-      </c>
       <c r="E12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G12" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" t="s">
         <v>48</v>
       </c>
-      <c r="B13" t="s">
-        <v>49</v>
-      </c>
       <c r="C13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E13" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F13" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G13" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D14" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E14" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G14" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>173</v>
+      </c>
+      <c r="B15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" t="s">
+        <v>92</v>
+      </c>
+      <c r="D15" t="s">
+        <v>129</v>
+      </c>
+      <c r="E15" t="s">
         <v>174</v>
-      </c>
-      <c r="B15" t="s">
-        <v>51</v>
-      </c>
-      <c r="C15" t="s">
-        <v>93</v>
-      </c>
-      <c r="D15" t="s">
-        <v>130</v>
-      </c>
-      <c r="E15" t="s">
-        <v>175</v>
       </c>
       <c r="G15" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="180" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D16" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E16" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G16" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E17" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F17" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G17" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D18" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E18" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G18" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D19" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E19" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G19" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C20" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D20" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E20" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F20" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G20" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="255" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="216" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E21" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G21" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>23</v>
+        <v>219</v>
       </c>
       <c r="B22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D22" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E22" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G22" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C23" t="s">
+        <v>182</v>
+      </c>
+      <c r="D23" t="s">
+        <v>137</v>
+      </c>
+      <c r="E23" t="s">
         <v>183</v>
       </c>
-      <c r="D23" t="s">
-        <v>138</v>
-      </c>
-      <c r="E23" t="s">
-        <v>184</v>
-      </c>
       <c r="F23" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G23" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D24" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E24" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G24" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D25" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E25" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G25" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C26" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D26" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E26" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G26" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="210" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C27" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D27" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E27" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G27" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C28" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D28" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F28" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G28" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="195" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C29" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D29" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E29" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G29" t="s">
         <v>3</v>
       </c>
       <c r="M29" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C30" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D30" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E30" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G30" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C31" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D31" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E31" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F31" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G31" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="375" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" ht="331.2" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C32" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D32" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E32" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F32" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G32" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C33" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D33" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E33" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G33" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="300" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B34" t="s">
         <v>69</v>
       </c>
-      <c r="B34" t="s">
-        <v>70</v>
-      </c>
       <c r="C34" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D34" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E34" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F34" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G34" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C35" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D35" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E35" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F35" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G35" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="180" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C36" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D36" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E36" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G36" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B37" t="s">
+        <v>72</v>
+      </c>
+      <c r="C37" t="s">
+        <v>112</v>
+      </c>
+      <c r="D37" t="s">
+        <v>151</v>
+      </c>
+      <c r="E37" t="s">
         <v>198</v>
-      </c>
-      <c r="B37" t="s">
-        <v>73</v>
-      </c>
-      <c r="C37" t="s">
-        <v>113</v>
-      </c>
-      <c r="D37" t="s">
-        <v>152</v>
-      </c>
-      <c r="E37" t="s">
-        <v>199</v>
       </c>
       <c r="G37" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="405" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="360" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B38" t="s">
         <v>74</v>
       </c>
-      <c r="B38" t="s">
-        <v>75</v>
-      </c>
       <c r="C38" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D38" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E38" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F38" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G38" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="330" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="288" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B39" t="s">
         <v>76</v>
       </c>
-      <c r="B39" t="s">
-        <v>77</v>
-      </c>
       <c r="C39" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D39" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E39" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F39" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G39" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
+        <v>201</v>
+      </c>
+      <c r="B40" t="s">
+        <v>77</v>
+      </c>
+      <c r="C40" t="s">
+        <v>115</v>
+      </c>
+      <c r="D40" t="s">
+        <v>154</v>
+      </c>
+      <c r="E40" t="s">
         <v>202</v>
       </c>
-      <c r="B40" t="s">
-        <v>78</v>
-      </c>
-      <c r="C40" t="s">
-        <v>116</v>
-      </c>
-      <c r="D40" t="s">
-        <v>155</v>
-      </c>
-      <c r="E40" t="s">
-        <v>203</v>
-      </c>
       <c r="F40" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G40" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="210" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B41" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C41" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D41" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E41" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G41" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>220</v>
+      </c>
+      <c r="B42" t="s">
+        <v>221</v>
+      </c>
+      <c r="C42" t="s">
+        <v>221</v>
+      </c>
+      <c r="D42" t="s">
+        <v>222</v>
+      </c>
+      <c r="E42" t="s">
+        <v>223</v>
+      </c>
+      <c r="F42" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B43" t="s">
+        <v>226</v>
+      </c>
+      <c r="C43" t="s">
+        <v>227</v>
+      </c>
+      <c r="D43" t="s">
+        <v>228</v>
+      </c>
+      <c r="E43" t="s">
+        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -1986,15 +2053,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000FBE23F23D6C404CAD5DE15B10DA803A" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9c0a2ea5eccded9113d6acc92c2e0eee">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="73decd86-39a4-49eb-910d-a9d7478bb842" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="95988c120be2346af9c3b7b357a780e1" ns3:_="">
     <xsd:import namespace="73decd86-39a4-49eb-910d-a9d7478bb842"/>
@@ -2152,6 +2210,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2159,14 +2226,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45F27491-F991-417B-A5F3-2092F2BFE652}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0CE6D41D-ABD0-43C8-8448-083F658CE12C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2180,6 +2239,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45F27491-F991-417B-A5F3-2092F2BFE652}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Finished quiz 6 and fixed the question class
</commit_message>
<xml_diff>
--- a/Stats Question.xlsx
+++ b/Stats Question.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pikak\CS\Stats_Study_Question\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02864EC5-6D84-4832-B072-1A2C2F496D29}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D325864C-F9E6-4E3B-8182-3D8BDBD2C836}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{E395EDCE-F408-40B2-8E9F-6BC6DF6B84F4}"/>
+    <workbookView xWindow="-14325" yWindow="3540" windowWidth="28800" windowHeight="15435" xr2:uid="{E395EDCE-F408-40B2-8E9F-6BC6DF6B84F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="244">
   <si>
     <t>Question</t>
   </si>
@@ -771,6 +771,52 @@
   </si>
   <si>
     <t>a probability sample.</t>
+  </si>
+  <si>
+    <t>Two essential features of all statistically designed experiments are that they</t>
+  </si>
+  <si>
+    <t>compare several treatments and use the double-blind method.</t>
+  </si>
+  <si>
+    <t>compare several treatments and use chance to assign subjects to treatments.</t>
+  </si>
+  <si>
+    <t>always have a placebo group and use the double-blind method.</t>
+  </si>
+  <si>
+    <t>use a block design and use chance to assign subjects to treatments.</t>
+  </si>
+  <si>
+    <t>A scientist is designing a clinical trial to test the effect of online chat counseling with migraine sufferers as a supplementary treatment in combating their migraines. Migraine sufferers will have access to counselors via online chat software; the scientist plans to see whether their migraine pain has been reduced after six weeks.
+Preliminary information suggests that the effect of (face-to-face) counseling is larger for migraine sufferers who are women than men. Knowing this, the scientist would probably use a</t>
+  </si>
+  <si>
+    <t>stratified random sample.</t>
+  </si>
+  <si>
+    <t>completely randomized design.</t>
+  </si>
+  <si>
+    <t>block design, with counseling and no counseling as the blocks.</t>
+  </si>
+  <si>
+    <t>block design, with women and men as the blocks</t>
+  </si>
+  <si>
+    <t>In order to take a sample of 1000 students at a college, a
+researcher first divides the students into freshmen, sophomores,
+juniors, and seniors, and then takes a simple random sample of 250
+students in each rank. This is an example of</t>
+  </si>
+  <si>
+    <t>a block design.</t>
+  </si>
+  <si>
+    <t>a stratified random sample.</t>
+  </si>
+  <si>
+    <t>a double-blind simple random sample</t>
   </si>
 </sst>
 </file>
@@ -786,15 +832,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -802,13 +860,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1125,930 +1200,1001 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A163365-0FC8-491B-B183-69C051A468D2}">
-  <dimension ref="A1:M43"/>
+  <dimension ref="A1:M46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="G50" sqref="G50"/>
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.109375" customWidth="1"/>
-    <col min="3" max="3" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="2"/>
+    <col min="5" max="5" width="9.140625" style="1"/>
+    <col min="6" max="6" width="9.140625" style="2"/>
+    <col min="7" max="7" width="9.140625" style="1"/>
+    <col min="12" max="12" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:7" ht="180" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G18" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G19" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G20" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="216" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
+    <row r="21" spans="1:13" ht="255" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G21" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
+    <row r="22" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G22" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G23" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G24" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="G25" t="s">
+      <c r="G25" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G26" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
+    <row r="27" spans="1:13" ht="210" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="G27" t="s">
+      <c r="G27" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F28" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G28" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
+    <row r="29" spans="1:13" ht="195" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="G29" t="s">
+      <c r="G29" s="1" t="s">
         <v>3</v>
       </c>
       <c r="M29" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="G30" t="s">
+      <c r="G30" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F31" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="G31" t="s">
+      <c r="G31" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="331.2" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
+    <row r="32" spans="1:13" ht="375" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F32" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="G32" t="s">
+      <c r="G32" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E33" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="G33" t="s">
+      <c r="G33" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="259.2" x14ac:dyDescent="0.3">
-      <c r="A34" s="1" t="s">
+    <row r="34" spans="1:7" ht="300" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E34" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="F34" t="s">
+      <c r="F34" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="G34" t="s">
+      <c r="G34" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A35" s="1" t="s">
+    <row r="35" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E35" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="F35" t="s">
+      <c r="F35" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="G35" t="s">
+      <c r="G35" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
+    <row r="36" spans="1:7" ht="180" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E36" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="G36" t="s">
+      <c r="G36" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A37" s="1" t="s">
+    <row r="37" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E37" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="G37" t="s">
+      <c r="G37" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="360" x14ac:dyDescent="0.3">
-      <c r="A38" s="1" t="s">
+    <row r="38" spans="1:7" ht="405" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E38" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F38" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="G38" t="s">
+      <c r="G38" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="288" x14ac:dyDescent="0.3">
-      <c r="A39" s="1" t="s">
+    <row r="39" spans="1:7" ht="330" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E39" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F39" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="G39" t="s">
+      <c r="G39" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E40" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F40" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="G40" t="s">
+      <c r="G40" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A41" s="1" t="s">
+    <row r="41" spans="1:7" ht="210" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E41" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="G41" t="s">
+      <c r="G41" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E42" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="F42" t="s">
+      <c r="F42" s="2" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A43" s="1" t="s">
+      <c r="G42" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D43" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E43" s="1" t="s">
         <v>229</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
created a way to most likely have different 15 questions until the set runs out
</commit_message>
<xml_diff>
--- a/Stats Question.xlsx
+++ b/Stats Question.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pikak\CS\Stats_Study_Question\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D325864C-F9E6-4E3B-8182-3D8BDBD2C836}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCFD04AC-6DC4-438D-8CB2-FAE0A83170B0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14325" yWindow="3540" windowWidth="28800" windowHeight="15435" xr2:uid="{E395EDCE-F408-40B2-8E9F-6BC6DF6B84F4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{E395EDCE-F408-40B2-8E9F-6BC6DF6B84F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="270">
   <si>
     <t>Question</t>
   </si>
@@ -817,6 +817,88 @@
   </si>
   <si>
     <t>a double-blind simple random sample</t>
+  </si>
+  <si>
+    <t>Over the past few years, college enrollments have increased dramatically across the United States. Over this same time period, an educational task force reports that the number of students dropping out of college has significantly increased.
+ A college newspaper reports on these results by stating, "In an effort to meet the demand of more students, it appears that colleges and universities are not providing the same level of support for students to graduate as they were a few years ago."
+What is wrong with the college newspaper's interpretation
+of the results?</t>
+  </si>
+  <si>
+    <t>Because more people attend college these days, one should expect that more people will drop out of college.</t>
+  </si>
+  <si>
+    <t>The newspaper is assuming that students drop out because of a lack of support.</t>
+  </si>
+  <si>
+    <t>Both A and B are correct.</t>
+  </si>
+  <si>
+    <t>Neither A nor B is correct.</t>
+  </si>
+  <si>
+    <t>How can one measure intelligence? One way is to measure the size of the brain. New technology makes it possible to measure the volume of a person's brain in cubic inches without injury. 
+What is more, the measurement gives close to the same answer when one repeats it. But how big the brain is has no relation to how smart a person is. As a measure of intelligence, brain volume is</t>
+  </si>
+  <si>
+    <t>reliable but invalid.</t>
+  </si>
+  <si>
+    <t>valid but not reliable.</t>
+  </si>
+  <si>
+    <t>valid and reliable.</t>
+  </si>
+  <si>
+    <t>not reliable and invalid</t>
+  </si>
+  <si>
+    <t>A student's research shows that there were more car accidents in 2015 than there were in 1915. He concludes that people were better drivers in 1915 than in 2015. Why is it not valid to use these two numbers to assess driving abilities in these 2 years?</t>
+  </si>
+  <si>
+    <t>People had more distractions on the road in 2010 than they had in 1910.</t>
+  </si>
+  <si>
+    <t>The numbers were compiled by a student instead of by a professional researcher.</t>
+  </si>
+  <si>
+    <t>The number of cars in the United States increased substantially from 1910 to 2010</t>
+  </si>
+  <si>
+    <t>One shouldn't compare years that are so far apart.</t>
+  </si>
+  <si>
+    <t>In an experiment to study the effect of vibrations on plant growth, the height of a chrysanthemum was measured three times. The reason for making the measurement three times instead of just once was probably to</t>
+  </si>
+  <si>
+    <t>decrease bias</t>
+  </si>
+  <si>
+    <t>eliminate confounding.</t>
+  </si>
+  <si>
+    <t>increase reliability</t>
+  </si>
+  <si>
+    <t>completely eliminate measurement error.</t>
+  </si>
+  <si>
+    <t>When repeated measurements each have a systematic error in the same direction, one says that the measurements contain</t>
+  </si>
+  <si>
+    <t>precision.</t>
+  </si>
+  <si>
+    <t>random error.</t>
+  </si>
+  <si>
+    <t>bias.</t>
+  </si>
+  <si>
+    <t>measurement error</t>
+  </si>
+  <si>
+    <t>observational studies generally cannot rule out confounding.</t>
   </si>
 </sst>
 </file>
@@ -1200,25 +1282,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A163365-0FC8-491B-B183-69C051A468D2}">
-  <dimension ref="A1:M46"/>
+  <dimension ref="A1:M51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="55.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="2"/>
-    <col min="5" max="5" width="9.140625" style="1"/>
-    <col min="6" max="6" width="9.140625" style="2"/>
-    <col min="7" max="7" width="9.140625" style="1"/>
-    <col min="12" max="12" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="19.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.109375" style="2"/>
+    <col min="5" max="5" width="9.109375" style="1"/>
+    <col min="6" max="6" width="9.109375" style="2"/>
+    <col min="7" max="7" width="9.109375" style="1"/>
+    <col min="12" max="12" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1241,7 +1323,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1261,7 +1343,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>157</v>
       </c>
@@ -1281,7 +1363,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1304,7 +1386,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>161</v>
       </c>
@@ -1324,7 +1406,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1347,7 +1429,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -1367,7 +1449,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -1387,7 +1469,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -1407,7 +1489,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
@@ -1430,7 +1512,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>13</v>
       </c>
@@ -1453,7 +1535,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
@@ -1473,7 +1555,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>47</v>
       </c>
@@ -1496,7 +1578,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
@@ -1516,7 +1598,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>173</v>
       </c>
@@ -1536,7 +1618,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="180" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>17</v>
       </c>
@@ -1556,7 +1638,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
@@ -1579,7 +1661,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -1599,7 +1681,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
@@ -1619,7 +1701,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
@@ -1642,7 +1724,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="255" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="216" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>22</v>
       </c>
@@ -1662,7 +1744,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>219</v>
       </c>
@@ -1682,7 +1764,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>23</v>
       </c>
@@ -1705,7 +1787,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
@@ -1725,7 +1807,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
@@ -1745,7 +1827,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>26</v>
       </c>
@@ -1765,7 +1847,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="210" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>27</v>
       </c>
@@ -1785,7 +1867,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>28</v>
       </c>
@@ -1805,7 +1887,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="195" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>29</v>
       </c>
@@ -1828,7 +1910,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>30</v>
       </c>
@@ -1848,7 +1930,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>31</v>
       </c>
@@ -1871,7 +1953,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="375" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" ht="331.2" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>32</v>
       </c>
@@ -1894,7 +1976,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>33</v>
       </c>
@@ -1914,7 +1996,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="300" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>68</v>
       </c>
@@ -1937,7 +2019,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>34</v>
       </c>
@@ -1960,7 +2042,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="180" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>35</v>
       </c>
@@ -1980,7 +2062,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>197</v>
       </c>
@@ -2000,7 +2082,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="405" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="360" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>73</v>
       </c>
@@ -2023,7 +2105,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="330" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="288" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>75</v>
       </c>
@@ -2046,7 +2128,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>201</v>
       </c>
@@ -2069,7 +2151,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="210" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>36</v>
       </c>
@@ -2089,7 +2171,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>220</v>
       </c>
@@ -2097,7 +2179,7 @@
         <v>221</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>221</v>
+        <v>269</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>222</v>
@@ -2112,7 +2194,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>225</v>
       </c>
@@ -2132,7 +2214,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>230</v>
       </c>
@@ -2152,7 +2234,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
         <v>235</v>
       </c>
@@ -2172,7 +2254,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>240</v>
       </c>
@@ -2190,6 +2272,103 @@
       </c>
       <c r="G46" s="1" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="144" x14ac:dyDescent="0.3">
+      <c r="A47" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A48" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A49" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -2199,6 +2378,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000FBE23F23D6C404CAD5DE15B10DA803A" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9c0a2ea5eccded9113d6acc92c2e0eee">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="73decd86-39a4-49eb-910d-a9d7478bb842" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="95988c120be2346af9c3b7b357a780e1" ns3:_="">
     <xsd:import namespace="73decd86-39a4-49eb-910d-a9d7478bb842"/>
@@ -2356,15 +2544,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2372,6 +2551,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45F27491-F991-417B-A5F3-2092F2BFE652}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0CE6D41D-ABD0-43C8-8448-083F658CE12C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2385,14 +2572,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45F27491-F991-417B-A5F3-2092F2BFE652}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
added all the questions
</commit_message>
<xml_diff>
--- a/Stats Question.xlsx
+++ b/Stats Question.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pikak\CS\Stats_Study_Question\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCFD04AC-6DC4-438D-8CB2-FAE0A83170B0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D944F7F3-B0B5-48AA-8023-6C9689A03A37}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{E395EDCE-F408-40B2-8E9F-6BC6DF6B84F4}"/>
+    <workbookView xWindow="-14325" yWindow="3540" windowWidth="28800" windowHeight="15435" xr2:uid="{E395EDCE-F408-40B2-8E9F-6BC6DF6B84F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="438">
   <si>
     <t>Question</t>
   </si>
@@ -899,6 +899,558 @@
   </si>
   <si>
     <t>observational studies generally cannot rule out confounding.</t>
+  </si>
+  <si>
+    <t>A 500-point drop in the DJIA was a big drop when the DJIA was at 2246 in October 1987 and a much smaller drop when the DJIA reached 11,421 in September 2008. 
+The percent by which stock prices fall is a more meaningful measure. The lesson here is that</t>
+  </si>
+  <si>
+    <t>rates are often more meaningful than counts</t>
+  </si>
+  <si>
+    <t>it is easy to make a mistake calculating a percent</t>
+  </si>
+  <si>
+    <t>the DJIA is a categorical variable.</t>
+  </si>
+  <si>
+    <t>confidentiality has been violated.</t>
+  </si>
+  <si>
+    <t>The value of a home decreased from $150,000 to $135,000.</t>
+  </si>
+  <si>
+    <t>This is a decrease of 15%.</t>
+  </si>
+  <si>
+    <t>This is a decrease of 10%.</t>
+  </si>
+  <si>
+    <t>This is a decrease of 1%</t>
+  </si>
+  <si>
+    <t>This is a decrease of 11%.</t>
+  </si>
+  <si>
+    <t>This is a decrease of 100%</t>
+  </si>
+  <si>
+    <t>A student reports that, of a simple random sample of 25 college undergraduate students, 18% were working at least two jobs. 
+We know that the student has made a mistake (or maybe really did not conduct the survey). Why?</t>
+  </si>
+  <si>
+    <t>There are 25 students in the sample, so percentages should be multiples of 0.04%.</t>
+  </si>
+  <si>
+    <t>There are 25 students in the sample, so percentages should be multiples of 4%.</t>
+  </si>
+  <si>
+    <t>18% of 25 students is 4.5 students, and you cannot sample a half of a student.</t>
+  </si>
+  <si>
+    <t>Both B and C are correct.</t>
+  </si>
+  <si>
+    <t>Which of the following statements do you think could possibly be true?</t>
+  </si>
+  <si>
+    <t>Last year, 60 of the 80 residents in a neighborhood subscribed to the local newspaper, and this year, it is 40 residents who subscribe. This is a 50% decrease.</t>
+  </si>
+  <si>
+    <t>A company's annual profits increased by 110% over the last decade.</t>
+  </si>
+  <si>
+    <t>A teacher brought 40 calculators to class, and 21% of them had dead batteries.</t>
+  </si>
+  <si>
+    <t>The number of violent crimes in the city decreased by 112.46% last year.</t>
+  </si>
+  <si>
+    <t>None of the above is true</t>
+  </si>
+  <si>
+    <t>The average wage of production workers (adjusted for the effects of inflation) was $11.08 an hour in 1981 and $10.35 an hour in 1991. In the decade of the 1980s, wages went down by about</t>
+  </si>
+  <si>
+    <t>73%.</t>
+  </si>
+  <si>
+    <t>7.3%.</t>
+  </si>
+  <si>
+    <t>7.0%.</t>
+  </si>
+  <si>
+    <t>6.6%.</t>
+  </si>
+  <si>
+    <t>Here is a table of the undergraduate enrollment at a large
+state university, broken down by class:
+Class: Freshman, Sophomore, Junior, Senior, Nondegree, Total
+Count of students: 8248, 8073, 7001, 6904, 535, 30,761 
+Percent of Students: 26.8%, 26.2%, 22.8%, 22.4%, 1.7%, 100%
+To make a correct graph of the distribution of students by class, you could use a</t>
+  </si>
+  <si>
+    <t>bar graph.</t>
+  </si>
+  <si>
+    <t>pie chart.</t>
+  </si>
+  <si>
+    <t>line graph.</t>
+  </si>
+  <si>
+    <t>Answers A, B, and C are correct</t>
+  </si>
+  <si>
+    <t>. Both A and B are correct.</t>
+  </si>
+  <si>
+    <t>it's the wrong kind of graph. Use a pie chart instead.</t>
+  </si>
+  <si>
+    <t>it's the wrong kind of graph. Use a scatterplot instead.</t>
+  </si>
+  <si>
+    <t>China's armed forces are twice as large as those of North Korea, but the choice of vertical scale can change this to half as large or four times as large.</t>
+  </si>
+  <si>
+    <t>China's armed forces are twice as large as those of North Korea, but the area of China's soldier picture is four times as large as the North Korea picture.</t>
+  </si>
+  <si>
+    <t>A line graph shows that the price of fresh oranges falls early in each year when the orange harvest in Florida is ready, 
+then it rises late in the year when oranges from that year's harvest begin to run out. This is an example of</t>
+  </si>
+  <si>
+    <t>A bar graph compares the size of the armed forces for China, North Korea, Russia, and the United States. To make the graph look nicer,
+ the artist replaces each bar by a proportionally correct picture of a soldier that is enlarged or reduced to be as tall as the bar. This graph is misleading because</t>
+  </si>
+  <si>
+    <t>trend in a line graph</t>
+  </si>
+  <si>
+    <t>erratic fluctuations in a line graph.</t>
+  </si>
+  <si>
+    <t>seasonal variation in a line graph.</t>
+  </si>
+  <si>
+    <t>confounding</t>
+  </si>
+  <si>
+    <t>A survey at a local university reveals that 30% of smartphone owners use Verizon, 45% use Sprint, and the remainder use a different company.
+A survey at a local university reveals that 30% of smartphone owners use Verizon, 45% use Sprint, and the remainder use a different company.</t>
+  </si>
+  <si>
+    <t>Were the extinctions that occurred in the last ice age more frequent among species of animals with large body sizes? A researcher gathers data on the average body mass (in kilograms) of all species known to have existed at that time. These measurements are values of</t>
+  </si>
+  <si>
+    <t>a categorical variable.</t>
+  </si>
+  <si>
+    <t>a quantitative variable.</t>
+  </si>
+  <si>
+    <t>an invalid variable.</t>
+  </si>
+  <si>
+    <t>a margin of error.</t>
+  </si>
+  <si>
+    <t>A stemplot is</t>
+  </si>
+  <si>
+    <t>the same as a boxplot.</t>
+  </si>
+  <si>
+    <t>a part of a small tree.</t>
+  </si>
+  <si>
+    <t>a picture of a distribution.</t>
+  </si>
+  <si>
+    <t>the same as a histogram.</t>
+  </si>
+  <si>
+    <t>useful for describing categorical variables.</t>
+  </si>
+  <si>
+    <t>To display the percent of likely voters who believe they are going to vote for a particular candidate according to a survey taken each week of an election year, 
+starting in January and ending the last week of October, a good choice of a graph would be a</t>
+  </si>
+  <si>
+    <t>boxplot.</t>
+  </si>
+  <si>
+    <t>histogram.</t>
+  </si>
+  <si>
+    <t>stemplot.</t>
+  </si>
+  <si>
+    <t>To display the number of pets owned by each of the 37 students in a class, a good choice of a graph would be a</t>
+  </si>
+  <si>
+    <t>According to a 2015 report by the New York Times and the Equilar 200 Highest-Paid CEO rankings, the median pay for these 200 CEOs was $17.6 million. 
+An examination of the pay distribution finds a handful to be very high (over a $100 million) with most "only" making eight-figure incomes. One would expect the mean to be</t>
+  </si>
+  <si>
+    <t>less than the median because salary distributions are skewed to the left.</t>
+  </si>
+  <si>
+    <t>less than the median because salary distributions are skewed to the right.</t>
+  </si>
+  <si>
+    <t>greater than the median because salary distributions are skewed to the left.</t>
+  </si>
+  <si>
+    <t>greater than the median because salary distributions are skewed to the right.</t>
+  </si>
+  <si>
+    <t>The possible values of the standard deviation s of a set of observations are</t>
+  </si>
+  <si>
+    <t>s can be any number, positive, 0, or negative.</t>
+  </si>
+  <si>
+    <t>s can be 0 or positive, but not negative.</t>
+  </si>
+  <si>
+    <t>s can be positive, but not 0 or negative.</t>
+  </si>
+  <si>
+    <t>s must be between –1 and 1</t>
+  </si>
+  <si>
+    <t>s must be between –1 and 1, but cannot be 0.</t>
+  </si>
+  <si>
+    <t>The following is a stemplot of 12 exam scores: (The stem is the tens place and the leaf is the ones place.)
+6|8
+7|66
+8|0488
+9|22666
+The first and third quartiles are, respectively,</t>
+  </si>
+  <si>
+    <t>The five numbers in the five-number summary are</t>
+  </si>
+  <si>
+    <t>76 and 92.</t>
+  </si>
+  <si>
+    <t>78 and 94.</t>
+  </si>
+  <si>
+    <t>94 and 78.</t>
+  </si>
+  <si>
+    <t>92 and 76.</t>
+  </si>
+  <si>
+    <t>None of the above</t>
+  </si>
+  <si>
+    <t>the five smallest observations.</t>
+  </si>
+  <si>
+    <t>the middle five observations.</t>
+  </si>
+  <si>
+    <t>the mean, the median, the maximum, the standard deviation, and the sample size.</t>
+  </si>
+  <si>
+    <t>x1, x2, x3, x4, and x5.</t>
+  </si>
+  <si>
+    <t>the median, the first quartile, the third quartile, the minimum, and the maximum.</t>
+  </si>
+  <si>
+    <t>Here are the number of text messages that each of a group of students sent during a recent statistics class:
+12 14 0 12 11 14 11 15 15 14
+The data contain one low outlier (0, or no text messages). Which of the results for the previous four questions would change if this were 10 messages instead of none?
+(There is no need to calculate new values.)</t>
+  </si>
+  <si>
+    <t>All four would change.</t>
+  </si>
+  <si>
+    <t>The mean, the third quartile, and the standard deviation would change.</t>
+  </si>
+  <si>
+    <t>The mean and the standard deviation would change.</t>
+  </si>
+  <si>
+    <t>Only the mean would change.</t>
+  </si>
+  <si>
+    <t>None of the four would change.</t>
+  </si>
+  <si>
+    <t>You measure the age (years), weight (pounds), and marital status (single, married, divorced, or widowed) of 1400 women. How many variables did you measure?</t>
+  </si>
+  <si>
+    <t>One</t>
+  </si>
+  <si>
+    <t>Two</t>
+  </si>
+  <si>
+    <t>Three</t>
+  </si>
+  <si>
+    <t>A statistics recitation has 30 students. The presenter wants to call a simple random sample (SRS) of five students 
+from the recitation to ask where they use a computer for the online exercises. The presenter labels the students 01, 02, …, 30 and enters the table of random digits at this line:
+09731 03453 76165 39241 87853 32459 26056 31424 80371 65103 62253 22490 61181
+The SRS contains the students labeled:</t>
+  </si>
+  <si>
+    <t>09, 73, 10, 34, 53.</t>
+  </si>
+  <si>
+    <t>09, 10, 34, 16, 24</t>
+  </si>
+  <si>
+    <t>09, 10, 16, 24, 26</t>
+  </si>
+  <si>
+    <t>09, 10, 16, 24, 24.</t>
+  </si>
+  <si>
+    <t>09, 07, 03, 10, 04.</t>
+  </si>
+  <si>
+    <t>An editorial writer for the East Mule Shoe Gazette wants to measure public support for a discontinued 
+construction project that has left a city-block-size hole in the middle of the East Mule Shoe downtown area, 
+so one day he uses his lunch hour to walk down the block adjacent to the project and interviews the first 25 people who will talk to him about it.
+The sample for this survey is</t>
+  </si>
+  <si>
+    <t>all residents of East Mule Shoe</t>
+  </si>
+  <si>
+    <t>all newspaper readers.</t>
+  </si>
+  <si>
+    <t>all people downtown the day the survey was conducted.</t>
+  </si>
+  <si>
+    <t>the 25 people who gave the editorial writer their opinion.</t>
+  </si>
+  <si>
+    <t>all American adults.</t>
+  </si>
+  <si>
+    <t>Professional sample surveys use careful random samples, usually by randomly dialing telephone numbers, to come close to an SRS. 
+But the results that a sample survey actually obtains may be strongly biased because</t>
+  </si>
+  <si>
+    <t>the typical sample size of 1000 or 1500 people is too small.</t>
+  </si>
+  <si>
+    <t>the margin of error is too large.</t>
+  </si>
+  <si>
+    <t>surveys report only what their sponsors want to hear</t>
+  </si>
+  <si>
+    <t>many people refuse to respond to telephone surveys</t>
+  </si>
+  <si>
+    <t>A Pew Research Council Poll recently showed that 23% of Americans are religiously unaffiliated and among these, 61% believe in God. 
+The poll contacted 35,071 adults by telephone. The margin of sampling error was plus or minus 0.6 (six-tenths) of a percentage point. 
+Assume a 95% confidence level and no bias. The numbers 23% and 61% in the report on the poll results are</t>
+  </si>
+  <si>
+    <t>parameters because they describe a population</t>
+  </si>
+  <si>
+    <t>parameters because they describe a sample.</t>
+  </si>
+  <si>
+    <t>statistics because they describe a population.</t>
+  </si>
+  <si>
+    <t>statistics because they describe a sample.</t>
+  </si>
+  <si>
+    <t>The margin of error for a poll is 4%. This means that</t>
+  </si>
+  <si>
+    <t>4% of those sampled did not answer the question asked.</t>
+  </si>
+  <si>
+    <t>there is a 95% confidence that the sample statistic is within 4% of the population parameter.</t>
+  </si>
+  <si>
+    <t>4% of those sampled gave the wrong answer to the question asked.</t>
+  </si>
+  <si>
+    <t>4% of the population was in the sample.</t>
+  </si>
+  <si>
+    <t>people's confidence in the statistic is 4%</t>
+  </si>
+  <si>
+    <t>The essential difference between an experiment and an observational study is that</t>
+  </si>
+  <si>
+    <t>observational studies always involve large numbers of subjects, but experiments never do</t>
+  </si>
+  <si>
+    <t>in an experiment, information is gathered only on animals or things, but in an observational study, only information about people is gathered.</t>
+  </si>
+  <si>
+    <t>an observational study imposes treatments on the subjects, but an experiment does not.</t>
+  </si>
+  <si>
+    <t>observational studies cannot have variables.</t>
+  </si>
+  <si>
+    <t>an experiment imposes treatments on the subjects, but an observational study does not.</t>
+  </si>
+  <si>
+    <t>The article was headlined, "Two Cups of Coffee Can Reduce the Risk of Liver Disease, Study Finds." 
+A metaanalysis, based on combining nine previous studies involving 430,000 individuals,
+ concluded that consumption of two cups of coffee a day reduced the chance of cirrhosis of the liver by 44 percent; 
+even greater consumption was found to further reduce the risk of the disease.
+The response variable in this study is:</t>
+  </si>
+  <si>
+    <t>incidence of cirrhosis of the liver.</t>
+  </si>
+  <si>
+    <t>coffee consumption.</t>
+  </si>
+  <si>
+    <t>no response variable because it is a meta-analysis.</t>
+  </si>
+  <si>
+    <t>not given in the quote above.</t>
+  </si>
+  <si>
+    <t>A sportswriter wants to know how strongly local residents support building a new stadium for the local minor league baseball team.
+She prints a survey in her column and asks her readers to send in their response. This is an example of</t>
+  </si>
+  <si>
+    <t>simple random sampling.</t>
+  </si>
+  <si>
+    <t>stratified sampling.</t>
+  </si>
+  <si>
+    <t>probability sampling.</t>
+  </si>
+  <si>
+    <t>voluntary response sampling.</t>
+  </si>
+  <si>
+    <t>A West Coast university statistics professor wishes to determine which surfboard brand delivers consistently longer rides, 
+Channel Island or JS. He recruits two of his students who surf to assist in an experiment, 
+and the student assigned to the Channel Island board is determined by coin flip. 
+The three head out to the beach for an afternoon, with the professor holding up a sign at random times for the respective student to catch the next wave on his board,
+ and the time spent on that wave is recorded. This is repeated until each student has ridden 10 waves.
+The brand of surfboard in this story is:</t>
+  </si>
+  <si>
+    <t>a parameter.</t>
+  </si>
+  <si>
+    <t>the response variable.</t>
+  </si>
+  <si>
+    <t>the explanatory variable</t>
+  </si>
+  <si>
+    <t>blinded.</t>
+  </si>
+  <si>
+    <t>stratified.</t>
+  </si>
+  <si>
+    <t>A poll about the effects of marijuana legalization questioned 1025 Denver residents and 472 Colorado citizens from outside Denver. 
+The design of the sample chose separate samples from the two groups and planned to interview more Denver residents than other Coloradans. This is a</t>
+  </si>
+  <si>
+    <t>systematic random sample.</t>
+  </si>
+  <si>
+    <t>census</t>
+  </si>
+  <si>
+    <t>simple random sample.</t>
+  </si>
+  <si>
+    <t>For a sample to be a simple random sample of size n,</t>
+  </si>
+  <si>
+    <t>the variability must be small.</t>
+  </si>
+  <si>
+    <t>n must be a large number.</t>
+  </si>
+  <si>
+    <t>every collection of n individuals must have the same chance to be the sample actually chosen.</t>
+  </si>
+  <si>
+    <t>the size of the population must be smaller than n.</t>
+  </si>
+  <si>
+    <t>The administration of Virginia Commonwealth University (VCU) has been asked to extend the
+ Drop/Add Period to two weeks (instead of the current one-week period). VCU will do so if it is convinced that more than 
+half of the student body is in favor of this change. Of the 1500 students surveyed, 803 are in favor of extending the Drop/Add Period as proposed.
+The response variable for this study is</t>
+  </si>
+  <si>
+    <t>1500 VCU students</t>
+  </si>
+  <si>
+    <t>803 VCU students.</t>
+  </si>
+  <si>
+    <t>number of classes surveyed.</t>
+  </si>
+  <si>
+    <t>opinion toward proposed change.</t>
+  </si>
+  <si>
+    <t>A table of random numbers is used to select 30 students from a statistics class to rate a statistics video.
+ The ratings that these students give are used to estimate the ratings that would be given if the entire class were asked to rate the video. This type of sample is</t>
+  </si>
+  <si>
+    <t>a biased sample.</t>
+  </si>
+  <si>
+    <t>a convenience sample.</t>
+  </si>
+  <si>
+    <t>a census.</t>
+  </si>
+  <si>
+    <t>voluntary response sample.</t>
+  </si>
+  <si>
+    <t>a sample that avoids bias.</t>
+  </si>
+  <si>
+    <t>Does coaching raise SAT scores? Because many students score higher on a second try, even without coaching, 
+a study looked at a simple random sample of 4200 students who took the SAT twice. Of these, 500 had taken coaching courses between their two attempts at the SAT. 
+The study compared the average increase in scores (out of the total possible score of 2400) for students who were coached with the average increase for students who were not coached.
+The study is 95% confident that the difference between average scores for coached and uncoached students
+is between 28 and 57 points. To be 99% confident, the range of points would be:</t>
+  </si>
+  <si>
+    <t>wider because higher confidence requires a larger margin of error</t>
+  </si>
+  <si>
+    <t>narrower because higher confidence requires a smaller margin of error.</t>
+  </si>
+  <si>
+    <t>wider because higher confidence requires a smaller margin of error.</t>
+  </si>
+  <si>
+    <t>narrower because higher confidence requires a larger margin of error</t>
   </si>
 </sst>
 </file>
@@ -961,13 +1513,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1282,25 +1840,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A163365-0FC8-491B-B183-69C051A468D2}">
-  <dimension ref="A1:M51"/>
+  <dimension ref="A1:M84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="H84" sqref="H84"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="19.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.109375" style="2"/>
-    <col min="5" max="5" width="9.109375" style="1"/>
-    <col min="6" max="6" width="9.109375" style="2"/>
-    <col min="7" max="7" width="9.109375" style="1"/>
-    <col min="12" max="12" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="2"/>
+    <col min="5" max="5" width="9.140625" style="1"/>
+    <col min="6" max="6" width="9.140625" style="2"/>
+    <col min="7" max="7" width="9.140625" style="1"/>
+    <col min="12" max="12" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1323,7 +1881,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1343,7 +1901,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>157</v>
       </c>
@@ -1363,7 +1921,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1386,7 +1944,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>161</v>
       </c>
@@ -1406,7 +1964,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1429,7 +1987,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -1449,7 +2007,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -1469,7 +2027,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -1489,7 +2047,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
@@ -1512,7 +2070,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>13</v>
       </c>
@@ -1535,7 +2093,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
@@ -1555,7 +2113,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>47</v>
       </c>
@@ -1578,7 +2136,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
@@ -1598,7 +2156,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>173</v>
       </c>
@@ -1618,7 +2176,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="180" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>17</v>
       </c>
@@ -1638,7 +2196,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
@@ -1661,7 +2219,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -1681,7 +2239,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
@@ -1701,7 +2259,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
@@ -1724,7 +2282,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="216" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" ht="255" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>22</v>
       </c>
@@ -1744,7 +2302,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>219</v>
       </c>
@@ -1764,7 +2322,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>23</v>
       </c>
@@ -1787,7 +2345,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
@@ -1807,7 +2365,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
@@ -1827,7 +2385,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>26</v>
       </c>
@@ -1847,7 +2405,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" ht="210" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>27</v>
       </c>
@@ -1867,7 +2425,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>28</v>
       </c>
@@ -1887,7 +2445,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" ht="195" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>29</v>
       </c>
@@ -1910,7 +2468,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>30</v>
       </c>
@@ -1930,7 +2488,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>31</v>
       </c>
@@ -1953,7 +2511,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="331.2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" ht="375" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>32</v>
       </c>
@@ -1976,7 +2534,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>33</v>
       </c>
@@ -1996,7 +2554,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" ht="300" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>68</v>
       </c>
@@ -2019,7 +2577,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>34</v>
       </c>
@@ -2042,7 +2600,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" ht="180" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>35</v>
       </c>
@@ -2062,7 +2620,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>197</v>
       </c>
@@ -2082,7 +2640,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="360" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" ht="405" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>73</v>
       </c>
@@ -2105,7 +2663,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="288" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" ht="330" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>75</v>
       </c>
@@ -2128,7 +2686,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>201</v>
       </c>
@@ -2151,7 +2709,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" ht="210" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>36</v>
       </c>
@@ -2171,7 +2729,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>220</v>
       </c>
@@ -2194,7 +2752,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>225</v>
       </c>
@@ -2214,7 +2772,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>230</v>
       </c>
@@ -2234,7 +2792,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>235</v>
       </c>
@@ -2254,7 +2812,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>240</v>
       </c>
@@ -2274,7 +2832,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="144" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" ht="180" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>244</v>
       </c>
@@ -2294,7 +2852,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>249</v>
       </c>
@@ -2311,7 +2869,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>254</v>
       </c>
@@ -2331,7 +2889,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>259</v>
       </c>
@@ -2351,7 +2909,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>264</v>
       </c>
@@ -2369,6 +2927,726 @@
       </c>
       <c r="G51" s="1" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="A57" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A58" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A59" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A60" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="B60" s="6">
+        <v>0.75</v>
+      </c>
+      <c r="C60" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="D60" s="6">
+        <v>0.7</v>
+      </c>
+      <c r="E60" s="7">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="F60" s="6">
+        <v>0.25</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="B65" s="6" t="s">
+        <v>331</v>
+      </c>
+      <c r="C65" s="7" t="s">
+        <v>332</v>
+      </c>
+      <c r="D65" s="6" t="s">
+        <v>333</v>
+      </c>
+      <c r="E65" s="7" t="s">
+        <v>334</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A67" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A69" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="B70" s="2">
+        <v>1400</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="F70" s="2">
+        <v>1403</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A71" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A72" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A73" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="G73" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A74" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="G74" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="G75" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="A77" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="G77" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A78" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="G78" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" ht="195" x14ac:dyDescent="0.25">
+      <c r="A79" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="G79" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A80" s="3" t="s">
+        <v>413</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="G80" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="G81" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="A82" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A83" s="3" t="s">
+        <v>427</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="F83" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="G83" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="195" x14ac:dyDescent="0.25">
+      <c r="A84" s="3" t="s">
+        <v>433</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="G84" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -2378,15 +3656,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000FBE23F23D6C404CAD5DE15B10DA803A" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9c0a2ea5eccded9113d6acc92c2e0eee">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="73decd86-39a4-49eb-910d-a9d7478bb842" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="95988c120be2346af9c3b7b357a780e1" ns3:_="">
     <xsd:import namespace="73decd86-39a4-49eb-910d-a9d7478bb842"/>
@@ -2544,6 +3813,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2551,14 +3829,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45F27491-F991-417B-A5F3-2092F2BFE652}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0CE6D41D-ABD0-43C8-8448-083F658CE12C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2572,6 +3842,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45F27491-F991-417B-A5F3-2092F2BFE652}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
fixed some error with the random int i think
</commit_message>
<xml_diff>
--- a/Stats Question.xlsx
+++ b/Stats Question.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pikak\CS\Stats_Study_Question\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D944F7F3-B0B5-48AA-8023-6C9689A03A37}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A20E8770-D2D9-41A9-8694-7D4AA6D19279}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14325" yWindow="3540" windowWidth="28800" windowHeight="15435" xr2:uid="{E395EDCE-F408-40B2-8E9F-6BC6DF6B84F4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{E395EDCE-F408-40B2-8E9F-6BC6DF6B84F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1842,23 +1842,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A163365-0FC8-491B-B183-69C051A468D2}">
   <dimension ref="A1:M84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="H84" sqref="H84"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="K57" sqref="K57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="55.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="2"/>
-    <col min="5" max="5" width="9.140625" style="1"/>
-    <col min="6" max="6" width="9.140625" style="2"/>
-    <col min="7" max="7" width="9.140625" style="1"/>
-    <col min="12" max="12" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="19.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.109375" style="2"/>
+    <col min="5" max="5" width="9.109375" style="1"/>
+    <col min="6" max="6" width="9.109375" style="2"/>
+    <col min="7" max="7" width="9.109375" style="1"/>
+    <col min="12" max="12" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1881,7 +1881,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1901,7 +1901,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>157</v>
       </c>
@@ -1921,7 +1921,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1944,7 +1944,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>161</v>
       </c>
@@ -1964,7 +1964,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1987,7 +1987,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -2007,7 +2007,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -2027,7 +2027,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -2047,7 +2047,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
@@ -2070,7 +2070,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>13</v>
       </c>
@@ -2093,7 +2093,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
@@ -2113,7 +2113,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>47</v>
       </c>
@@ -2136,7 +2136,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
@@ -2156,7 +2156,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>173</v>
       </c>
@@ -2176,7 +2176,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="180" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>17</v>
       </c>
@@ -2196,7 +2196,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
@@ -2219,7 +2219,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -2239,7 +2239,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
@@ -2259,7 +2259,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
@@ -2282,7 +2282,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="255" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="216" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>22</v>
       </c>
@@ -2302,7 +2302,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>219</v>
       </c>
@@ -2322,7 +2322,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>23</v>
       </c>
@@ -2345,7 +2345,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
@@ -2365,7 +2365,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
@@ -2385,7 +2385,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>26</v>
       </c>
@@ -2405,7 +2405,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="210" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>27</v>
       </c>
@@ -2425,7 +2425,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>28</v>
       </c>
@@ -2445,7 +2445,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="195" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>29</v>
       </c>
@@ -2468,7 +2468,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>30</v>
       </c>
@@ -2488,7 +2488,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>31</v>
       </c>
@@ -2511,7 +2511,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="375" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" ht="331.2" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>32</v>
       </c>
@@ -2534,7 +2534,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>33</v>
       </c>
@@ -2554,7 +2554,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="300" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>68</v>
       </c>
@@ -2577,7 +2577,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>34</v>
       </c>
@@ -2600,7 +2600,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="180" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>35</v>
       </c>
@@ -2620,7 +2620,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>197</v>
       </c>
@@ -2640,7 +2640,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="405" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="360" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>73</v>
       </c>
@@ -2663,7 +2663,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="330" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="288" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>75</v>
       </c>
@@ -2686,7 +2686,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>201</v>
       </c>
@@ -2709,7 +2709,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="210" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>36</v>
       </c>
@@ -2729,7 +2729,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>220</v>
       </c>
@@ -2752,7 +2752,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>225</v>
       </c>
@@ -2772,7 +2772,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>230</v>
       </c>
@@ -2792,7 +2792,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
         <v>235</v>
       </c>
@@ -2812,7 +2812,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>240</v>
       </c>
@@ -2832,7 +2832,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="180" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" ht="144" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
         <v>244</v>
       </c>
@@ -2852,7 +2852,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>249</v>
       </c>
@@ -2869,7 +2869,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>254</v>
       </c>
@@ -2889,7 +2889,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>259</v>
       </c>
@@ -2909,7 +2909,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>264</v>
       </c>
@@ -2929,7 +2929,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
         <v>270</v>
       </c>
@@ -2949,7 +2949,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>275</v>
       </c>
@@ -2972,7 +2972,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
         <v>281</v>
       </c>
@@ -2995,7 +2995,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>286</v>
       </c>
@@ -3018,7 +3018,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>292</v>
       </c>
@@ -3038,7 +3038,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
         <v>297</v>
       </c>
@@ -3061,7 +3061,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
         <v>308</v>
       </c>
@@ -3081,7 +3081,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
         <v>307</v>
       </c>
@@ -3101,7 +3101,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
         <v>313</v>
       </c>
@@ -3124,7 +3124,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>314</v>
       </c>
@@ -3144,7 +3144,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>319</v>
       </c>
@@ -3167,7 +3167,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
         <v>325</v>
       </c>
@@ -3190,7 +3190,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>329</v>
       </c>
@@ -3213,7 +3213,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
         <v>330</v>
       </c>
@@ -3233,7 +3233,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>335</v>
       </c>
@@ -3256,7 +3256,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
         <v>341</v>
       </c>
@@ -3279,7 +3279,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>342</v>
       </c>
@@ -3302,7 +3302,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
         <v>353</v>
       </c>
@@ -3325,7 +3325,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>359</v>
       </c>
@@ -3348,7 +3348,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
         <v>363</v>
       </c>
@@ -3371,7 +3371,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="s">
         <v>369</v>
       </c>
@@ -3394,7 +3394,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
         <v>375</v>
       </c>
@@ -3414,7 +3414,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A74" s="3" t="s">
         <v>380</v>
       </c>
@@ -3434,7 +3434,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>385</v>
       </c>
@@ -3457,7 +3457,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>391</v>
       </c>
@@ -3480,7 +3480,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="s">
         <v>397</v>
       </c>
@@ -3500,7 +3500,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
         <v>402</v>
       </c>
@@ -3520,7 +3520,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="195" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="s">
         <v>407</v>
       </c>
@@ -3543,7 +3543,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A80" s="3" t="s">
         <v>413</v>
       </c>
@@ -3563,7 +3563,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>417</v>
       </c>
@@ -3586,7 +3586,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A82" s="3" t="s">
         <v>422</v>
       </c>
@@ -3606,7 +3606,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A83" s="3" t="s">
         <v>427</v>
       </c>
@@ -3629,7 +3629,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="195" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A84" s="3" t="s">
         <v>433</v>
       </c>
@@ -3656,6 +3656,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000FBE23F23D6C404CAD5DE15B10DA803A" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9c0a2ea5eccded9113d6acc92c2e0eee">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="73decd86-39a4-49eb-910d-a9d7478bb842" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="95988c120be2346af9c3b7b357a780e1" ns3:_="">
     <xsd:import namespace="73decd86-39a4-49eb-910d-a9d7478bb842"/>
@@ -3813,15 +3822,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -3829,6 +3829,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45F27491-F991-417B-A5F3-2092F2BFE652}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0CE6D41D-ABD0-43C8-8448-083F658CE12C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3842,14 +3850,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45F27491-F991-417B-A5F3-2092F2BFE652}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>